<commit_message>
Sistmea de chamados upgrade
</commit_message>
<xml_diff>
--- a/compras/gerar_relatorio_categorias_2024.xlsx
+++ b/compras/gerar_relatorio_categorias_2024.xlsx
@@ -551,8 +551,8 @@
     <col min="6" max="6" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="11.569" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="12.854" bestFit="true" customWidth="true" style="0"/>
@@ -627,15 +627,17 @@
         <v>6746.59</v>
       </c>
       <c r="H3" s="5">
-        <v>4956.59</v>
-      </c>
-      <c r="I3" s="5"/>
+        <v>5893.22</v>
+      </c>
+      <c r="I3" s="5">
+        <v>5642.72</v>
+      </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="6">
-        <v>23625.63</v>
+        <v>30204.98</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -658,14 +660,14 @@
         <v>7374.38</v>
       </c>
       <c r="I4" s="5">
-        <v>945.0</v>
+        <v>11199.23</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="6">
-        <v>63877.75</v>
+        <v>74131.98</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -772,14 +774,14 @@
         <v>6720.01</v>
       </c>
       <c r="I8" s="5">
-        <v>3131.63</v>
+        <v>10096.28</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="6">
-        <v>24575.84</v>
+        <v>31540.49</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -802,14 +804,16 @@
         <v>99.0</v>
       </c>
       <c r="I9" s="5">
-        <v>1053.68</v>
-      </c>
-      <c r="J9" s="5"/>
+        <v>1294.43</v>
+      </c>
+      <c r="J9" s="5">
+        <v>102.8</v>
+      </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="6">
-        <v>11139.45</v>
+        <v>11483.0</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -851,17 +855,19 @@
         <v>19958.54</v>
       </c>
       <c r="H11" s="8">
-        <v>22003.63</v>
+        <v>22940.26</v>
       </c>
       <c r="I11" s="8">
-        <v>5352.21</v>
-      </c>
-      <c r="J11" s="8"/>
+        <v>28454.56</v>
+      </c>
+      <c r="J11" s="8">
+        <v>102.8</v>
+      </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="6">
-        <v>137159.18</v>
+        <v>161300.96</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -930,15 +936,17 @@
         <v>4669.0</v>
       </c>
       <c r="H15" s="5">
-        <v>2634.49</v>
-      </c>
-      <c r="I15" s="5"/>
+        <v>3471.47</v>
+      </c>
+      <c r="I15" s="5">
+        <v>2627.34</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="6">
-        <v>23625.63</v>
+        <v>30204.98</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1030,7 +1038,7 @@
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="6">
-        <v>24575.84</v>
+        <v>31540.49</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1050,13 +1058,15 @@
       <c r="H20" s="5">
         <v>379.6</v>
       </c>
-      <c r="I20" s="5"/>
+      <c r="I20" s="5">
+        <v>379.6</v>
+      </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="6">
-        <v>11139.45</v>
+        <v>11483.0</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1076,15 +1086,17 @@
         <v>6643.08</v>
       </c>
       <c r="H21" s="8">
-        <v>3014.09</v>
-      </c>
-      <c r="I21" s="8"/>
+        <v>3851.07</v>
+      </c>
+      <c r="I21" s="8">
+        <v>3006.94</v>
+      </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="6">
-        <v>28252.08</v>
+        <v>32096.0</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1155,13 +1167,15 @@
       <c r="H25" s="5">
         <v>1339.85</v>
       </c>
-      <c r="I25" s="5"/>
+      <c r="I25" s="5">
+        <v>355.66</v>
+      </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="6">
-        <v>23625.63</v>
+        <v>30204.98</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1183,7 +1197,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="6">
-        <v>24575.84</v>
+        <v>31540.49</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1205,7 +1219,7 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="6">
-        <v>11139.45</v>
+        <v>11483.0</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -1227,13 +1241,15 @@
       <c r="H28" s="8">
         <v>1624.55</v>
       </c>
-      <c r="I28" s="8"/>
+      <c r="I28" s="8">
+        <v>355.66</v>
+      </c>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
       <c r="N28" s="6">
-        <v>3950.59</v>
+        <v>4306.25</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -1304,7 +1320,9 @@
       <c r="H32" s="5">
         <v>43986.83</v>
       </c>
-      <c r="I32" s="5"/>
+      <c r="I32" s="5">
+        <v>18677.34</v>
+      </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -1370,7 +1388,7 @@
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
       <c r="N35" s="6">
-        <v>23625.63</v>
+        <v>30204.98</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -1414,13 +1432,15 @@
       <c r="H37" s="11">
         <v>44741.83</v>
       </c>
-      <c r="I37" s="11"/>
+      <c r="I37" s="11">
+        <v>18677.34</v>
+      </c>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
       <c r="N37" s="6">
-        <v>70337.32</v>
+        <v>89014.66</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -1491,7 +1511,9 @@
       <c r="H41" s="5">
         <v>9877.74</v>
       </c>
-      <c r="I41" s="5"/>
+      <c r="I41" s="5">
+        <v>8590.23</v>
+      </c>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
@@ -1517,13 +1539,15 @@
       <c r="H42" s="11">
         <v>9877.74</v>
       </c>
-      <c r="I42" s="11"/>
+      <c r="I42" s="11">
+        <v>8590.23</v>
+      </c>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
       <c r="L42" s="11"/>
       <c r="M42" s="11"/>
       <c r="N42" s="6">
-        <v>16085.25</v>
+        <v>24675.48</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -1590,9 +1614,11 @@
         <v>719.7</v>
       </c>
       <c r="H46" s="5">
-        <v>7206.23</v>
-      </c>
-      <c r="I46" s="5"/>
+        <v>7663.68</v>
+      </c>
+      <c r="I46" s="5">
+        <v>4452.6</v>
+      </c>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
@@ -1614,15 +1640,17 @@
         <v>719.7</v>
       </c>
       <c r="H47" s="11">
-        <v>7206.23</v>
-      </c>
-      <c r="I47" s="11"/>
+        <v>7663.68</v>
+      </c>
+      <c r="I47" s="11">
+        <v>4452.6</v>
+      </c>
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
       <c r="L47" s="11"/>
       <c r="M47" s="11"/>
       <c r="N47" s="6">
-        <v>8637.24</v>
+        <v>13547.29</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -1630,7 +1658,7 @@
         <v>31</v>
       </c>
       <c r="B50" s="5">
-        <v>170292.18</v>
+        <v>198633.54</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -1638,7 +1666,7 @@
         <v>32</v>
       </c>
       <c r="B51" s="5">
-        <v>95059.81</v>
+        <v>127237.43</v>
       </c>
     </row>
   </sheetData>
@@ -1844,6 +1872,9 @@
       <c r="T4">
         <v>299.0</v>
       </c>
+      <c r="W4">
+        <v>176.0</v>
+      </c>
     </row>
     <row r="5" spans="1:37">
       <c r="A5" t="s">
@@ -1907,7 +1938,9 @@
       </c>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
+      <c r="W9" s="10">
+        <v>176.0</v>
+      </c>
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
@@ -2095,6 +2128,9 @@
       <c r="T14">
         <v>92.0</v>
       </c>
+      <c r="W14">
+        <v>101.0</v>
+      </c>
     </row>
     <row r="15" spans="1:37">
       <c r="A15" t="s">
@@ -2149,7 +2185,9 @@
       </c>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
+      <c r="W19" s="10">
+        <v>101.0</v>
+      </c>
       <c r="X19" s="10"/>
       <c r="Y19" s="10"/>
       <c r="Z19" s="10"/>
@@ -2332,7 +2370,10 @@
         <v>10.0</v>
       </c>
       <c r="T24">
-        <v>55.0</v>
+        <v>57.0</v>
+      </c>
+      <c r="W24">
+        <v>63.0</v>
       </c>
     </row>
     <row r="25" spans="1:37">
@@ -2382,11 +2423,13 @@
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
       <c r="T29" s="10">
-        <v>55.0</v>
+        <v>57.0</v>
       </c>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
-      <c r="W29" s="10"/>
+      <c r="W29" s="10">
+        <v>63.0</v>
+      </c>
       <c r="X29" s="10"/>
       <c r="Y29" s="10"/>
       <c r="Z29" s="10"/>

</xml_diff>

<commit_message>
atualização 2.0 relatório notas_fiscais
</commit_message>
<xml_diff>
--- a/compras/gerar_relatorio_categorias_2024.xlsx
+++ b/compras/gerar_relatorio_categorias_2024.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Valor" sheetId="1" r:id="rId4"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>RELATORIO RESUMO GERAL CLINICA PARQUE - 2024</t>
   </si>
@@ -60,34 +60,37 @@
     <t>DEZEMBRO</t>
   </si>
   <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>ATIVO FIXO</t>
+  </si>
+  <si>
+    <t>LENTE DE CONTATO</t>
+  </si>
+  <si>
+    <t>LENTE INTRAOCULAR</t>
+  </si>
+  <si>
+    <t>MANUTENçãO DE EQUIPAMENTOS</t>
+  </si>
+  <si>
+    <t>MANUTENçãO PREDIAL</t>
+  </si>
+  <si>
+    <t>MATERIAIS DE ESCRITORIO</t>
+  </si>
+  <si>
+    <t>MEDICAMENTOS / MATERIAL HOSPITALAR</t>
+  </si>
+  <si>
+    <t>PRODUTOS DE LIMPEZA</t>
+  </si>
+  <si>
+    <t>UNIFORME</t>
+  </si>
+  <si>
     <t>TOTAL:</t>
-  </si>
-  <si>
-    <t>ATIVO FIXO</t>
-  </si>
-  <si>
-    <t>LENTE DE CONTATO</t>
-  </si>
-  <si>
-    <t>LENTE INTRAOCULAR</t>
-  </si>
-  <si>
-    <t>MANUTENçãO DE EQUIPAMENTOS</t>
-  </si>
-  <si>
-    <t>MANUTENçãO PREDIAL</t>
-  </si>
-  <si>
-    <t>MATERIAIS DE ESCRITORIO</t>
-  </si>
-  <si>
-    <t>MEDICAMENTOS / MATERIAL HOSPITALAR</t>
-  </si>
-  <si>
-    <t>PRODUTOS DE LIMPEZA</t>
-  </si>
-  <si>
-    <t>UNIFORME</t>
   </si>
   <si>
     <t>RELATORIO RESUMO GERAL CLINICA MAUÁ - 2024</t>
@@ -145,13 +148,22 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-R$* #,##0.00_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -174,7 +186,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,30 +195,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4682B4"/>
+        <fgColor rgb="FF538DD5"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFADD8E6"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF32CD32"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF98FB98"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -214,31 +220,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="2" numFmtId="164" fillId="3" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="3" numFmtId="164" fillId="0" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="3" numFmtId="164" fillId="3" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="164" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="2" numFmtId="164" fillId="0" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="164" fillId="3" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="5" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="164" fillId="5" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="2" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="4" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="2" numFmtId="164" fillId="4" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,7 +567,7 @@
   </sheetPr>
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
@@ -568,53 +595,66 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="5"/>
@@ -633,12 +673,12 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="6">
+      <c r="N3" s="7">
         <v>1383.0</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="5"/>
@@ -665,12 +705,12 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="6">
+      <c r="N4" s="7">
         <v>33885.64</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="5"/>
@@ -697,12 +737,12 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="6">
+      <c r="N5" s="7">
         <v>121950.78</v>
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="5"/>
@@ -729,12 +769,12 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="6">
+      <c r="N6" s="7">
         <v>5202.06</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="5"/>
@@ -757,12 +797,12 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="6">
+      <c r="N7" s="7">
         <v>5637.72</v>
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="5"/>
@@ -787,12 +827,12 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="6">
+      <c r="N8" s="7">
         <v>9866.07</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="5"/>
@@ -819,12 +859,12 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="6">
+      <c r="N9" s="7">
         <v>38027.25</v>
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="5"/>
@@ -851,12 +891,12 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="6">
+      <c r="N10" s="7">
         <v>11483.0</v>
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="5"/>
@@ -873,93 +913,106 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="6">
+      <c r="N11" s="7">
         <v>879.56</v>
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6">
         <v>18872.96</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <v>70971.84</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="6">
         <v>19958.54</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="6">
         <v>22940.26</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="6">
         <v>75858.36</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="6">
         <v>19713.12</v>
       </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="6">
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="8">
         <v>228315.08</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="5"/>
@@ -986,12 +1039,12 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="6">
+      <c r="N16" s="7">
         <v>33885.64</v>
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="5"/>
@@ -1008,12 +1061,12 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
-      <c r="N17" s="6">
+      <c r="N17" s="7">
         <v>5202.06</v>
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="5"/>
@@ -1034,12 +1087,12 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
-      <c r="N18" s="6">
+      <c r="N18" s="7">
         <v>5637.72</v>
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="5"/>
@@ -1056,12 +1109,12 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="6">
+      <c r="N19" s="7">
         <v>9866.07</v>
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="5"/>
@@ -1078,12 +1131,12 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-      <c r="N20" s="6">
+      <c r="N20" s="7">
         <v>38027.25</v>
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="5"/>
@@ -1106,93 +1159,106 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
-      <c r="N21" s="6">
+      <c r="N21" s="7">
         <v>11483.0</v>
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6">
         <v>5304.24</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="6">
         <v>13290.67</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="6">
         <v>6643.08</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="6">
         <v>3851.07</v>
       </c>
-      <c r="I22" s="8">
+      <c r="I22" s="6">
         <v>3006.94</v>
       </c>
-      <c r="J22" s="8">
+      <c r="J22" s="6">
         <v>3172.91</v>
       </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="6">
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="8">
         <v>35268.91</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="L25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M25" s="4" t="s">
+      <c r="M25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="5"/>
@@ -1219,12 +1285,12 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
-      <c r="N26" s="6">
+      <c r="N26" s="7">
         <v>33885.64</v>
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="5"/>
@@ -1241,12 +1307,12 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
-      <c r="N27" s="6">
+      <c r="N27" s="7">
         <v>38027.25</v>
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="5"/>
@@ -1265,94 +1331,107 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
-      <c r="N28" s="6">
+      <c r="N28" s="7">
         <v>11483.0</v>
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8">
+      <c r="A29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6">
         <v>915.7</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="6">
         <v>632.38</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="6">
         <v>777.96</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="6">
         <v>1624.55</v>
       </c>
-      <c r="I29" s="8">
+      <c r="I29" s="6">
         <v>355.66</v>
       </c>
-      <c r="J29" s="8">
+      <c r="J29" s="6">
         <v>561.06</v>
       </c>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="6">
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="8">
         <v>4867.31</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="9" t="s">
-        <v>26</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H32" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J32" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="L32" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="4" t="s">
+      <c r="M32" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="N32" t="s">
+      <c r="N32" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" t="s">
-        <v>27</v>
+      <c r="A33" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1378,11 +1457,11 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
-      <c r="N33" s="6"/>
+      <c r="N33" s="7"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" t="s">
-        <v>28</v>
+      <c r="A34" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1398,11 +1477,11 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="6"/>
+      <c r="N34" s="7"/>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" t="s">
-        <v>29</v>
+      <c r="A35" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1418,10 +1497,10 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
-      <c r="N35" s="6"/>
+      <c r="N35" s="7"/>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" t="s">
+      <c r="A36" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="5"/>
@@ -1438,12 +1517,12 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
-      <c r="N36" s="6">
+      <c r="N36" s="7">
         <v>33885.64</v>
       </c>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" t="s">
+      <c r="A37" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B37" s="5"/>
@@ -1460,94 +1539,107 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
-      <c r="N37" s="6">
+      <c r="N37" s="7">
         <v>9866.07</v>
       </c>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11">
+      <c r="A38" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6">
         <v>6999.52</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F38" s="6">
         <v>11999.86</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="6">
         <v>6596.11</v>
       </c>
-      <c r="H38" s="11">
+      <c r="H38" s="6">
         <v>44741.83</v>
       </c>
-      <c r="I38" s="11">
+      <c r="I38" s="6">
         <v>18677.34</v>
       </c>
-      <c r="J38" s="11">
+      <c r="J38" s="6">
         <v>2191.99</v>
       </c>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="6">
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="8">
         <v>91206.65</v>
       </c>
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:16">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="H41" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="I41" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="J41" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="K41" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L41" s="4" t="s">
+      <c r="L41" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M41" s="4" t="s">
+      <c r="M41" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N41" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:16">
-      <c r="A42" t="s">
-        <v>27</v>
+      <c r="A42" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1571,11 +1663,11 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
-      <c r="N42" s="6"/>
+      <c r="N42" s="7"/>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" t="s">
-        <v>29</v>
+      <c r="A43" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1591,92 +1683,105 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
-      <c r="N43" s="6"/>
+      <c r="N43" s="7"/>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11">
+      <c r="A44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6">
         <v>1448.82</v>
       </c>
-      <c r="F44" s="11">
+      <c r="F44" s="6">
         <v>3814.76</v>
       </c>
-      <c r="G44" s="11">
+      <c r="G44" s="6">
         <v>943.93</v>
       </c>
-      <c r="H44" s="11">
+      <c r="H44" s="6">
         <v>9877.74</v>
       </c>
-      <c r="I44" s="11">
+      <c r="I44" s="6">
         <v>8730.98</v>
       </c>
-      <c r="J44" s="11">
+      <c r="J44" s="6">
         <v>473.01</v>
       </c>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-      <c r="N44" s="6">
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="8">
         <v>25289.24</v>
       </c>
     </row>
     <row r="46" spans="1:16">
       <c r="A46" s="9" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F47" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="G47" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="H47" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="I47" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="J47" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K47" s="4" t="s">
+      <c r="K47" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L47" s="4" t="s">
+      <c r="L47" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M47" s="4" t="s">
+      <c r="M47" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="N47" t="s">
+      <c r="N47" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:16">
-      <c r="A48" t="s">
-        <v>27</v>
+      <c r="A48" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -1700,11 +1805,11 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
-      <c r="N48" s="6"/>
+      <c r="N48" s="7"/>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" t="s">
-        <v>29</v>
+      <c r="A49" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -1720,51 +1825,51 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
       <c r="M49" s="5"/>
-      <c r="N49" s="6"/>
+      <c r="N49" s="7"/>
     </row>
     <row r="50" spans="1:16">
-      <c r="A50" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11">
+      <c r="A50" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6">
         <v>711.31</v>
       </c>
-      <c r="G50" s="11">
+      <c r="G50" s="6">
         <v>719.7</v>
       </c>
-      <c r="H50" s="11">
+      <c r="H50" s="6">
         <v>7663.68</v>
       </c>
-      <c r="I50" s="11">
+      <c r="I50" s="6">
         <v>4452.6</v>
       </c>
-      <c r="J50" s="11">
+      <c r="J50" s="6">
         <v>1760.39</v>
       </c>
-      <c r="K50" s="11"/>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11"/>
-      <c r="N50" s="6">
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="8">
         <v>15307.68</v>
       </c>
     </row>
     <row r="53" spans="1:16">
-      <c r="A53" t="s">
-        <v>32</v>
-      </c>
-      <c r="B53" s="5">
+      <c r="A53" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="12">
         <v>269765.63</v>
       </c>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" t="s">
-        <v>33</v>
-      </c>
-      <c r="B54" s="5">
+      <c r="A54" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" s="14">
         <v>131803.57</v>
       </c>
     </row>
@@ -1791,7 +1896,7 @@
   <dimension ref="A1:AK29"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AK29" sqref="AK29"/>
+      <selection activeCell="A21" sqref="A21:AK29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1801,766 +1906,1468 @@
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1" s="9" t="s">
-        <v>34</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
     </row>
     <row r="2" spans="1:37">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
     </row>
     <row r="3" spans="1:37">
-      <c r="B3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>37</v>
+      <c r="A3" s="3"/>
+      <c r="B3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK3" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:37">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4">
+      <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3">
         <v>5.0</v>
       </c>
-      <c r="N4">
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3">
         <v>54.0</v>
       </c>
-      <c r="Q4">
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3">
         <v>70.0</v>
       </c>
-      <c r="T4">
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3">
         <v>299.0</v>
       </c>
-      <c r="W4">
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3">
         <v>176.0</v>
       </c>
-      <c r="Z4">
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3">
         <v>76.0</v>
       </c>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3"/>
     </row>
     <row r="5" spans="1:37">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
     </row>
     <row r="6" spans="1:37">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T6">
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3">
         <v>1.0</v>
       </c>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
     </row>
     <row r="7" spans="1:37">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N7">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3">
         <v>3.0</v>
       </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
     </row>
     <row r="8" spans="1:37">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3">
         <v>1.0</v>
       </c>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
     </row>
     <row r="9" spans="1:37">
-      <c r="A9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10">
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4">
         <v>5.0</v>
       </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10">
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4">
         <v>57.0</v>
       </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10">
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4">
         <v>71.0</v>
       </c>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10">
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4">
         <v>300.0</v>
       </c>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10">
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4">
         <v>176.0</v>
       </c>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="10">
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4">
         <v>76.0</v>
       </c>
-      <c r="AA9" s="10"/>
-      <c r="AB9" s="10"/>
-      <c r="AC9" s="10"/>
-      <c r="AD9" s="10"/>
-      <c r="AE9" s="10"/>
-      <c r="AF9" s="10"/>
-      <c r="AG9" s="10"/>
-      <c r="AH9" s="10"/>
-      <c r="AI9" s="10"/>
-      <c r="AJ9" s="10"/>
-      <c r="AK9" s="10"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="4"/>
     </row>
     <row r="11" spans="1:37">
       <c r="A11" s="9" t="s">
-        <v>38</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
     </row>
     <row r="12" spans="1:37">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="T12" s="4" t="s">
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="W12" s="4" t="s">
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Z12" s="4" t="s">
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AC12" s="4" t="s">
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AF12" s="4" t="s">
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI12" s="4" t="s">
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
     </row>
     <row r="13" spans="1:37">
-      <c r="B13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK13" s="3" t="s">
-        <v>37</v>
+      <c r="A13" s="3"/>
+      <c r="B13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="P13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="R13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="T13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="U13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="V13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="W13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="X13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK13" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:37">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="K14">
+      <c r="A14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3">
         <v>3.0</v>
       </c>
-      <c r="N14">
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3">
         <v>12.0</v>
       </c>
-      <c r="Q14">
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3">
         <v>12.0</v>
       </c>
-      <c r="T14">
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3">
         <v>92.0</v>
       </c>
-      <c r="W14">
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3">
         <v>102.0</v>
       </c>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3"/>
     </row>
     <row r="15" spans="1:37">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
+      <c r="A15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3"/>
+      <c r="AK15" s="3"/>
     </row>
     <row r="16" spans="1:37">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z16">
+      <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3">
         <v>1.0</v>
       </c>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="3"/>
     </row>
     <row r="17" spans="1:37">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
+      <c r="AK17" s="3"/>
     </row>
     <row r="18" spans="1:37">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3"/>
     </row>
     <row r="19" spans="1:37">
-      <c r="A19" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4">
         <v>3.0</v>
       </c>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10">
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4">
         <v>12.0</v>
       </c>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10">
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4">
         <v>12.0</v>
       </c>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10">
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4">
         <v>92.0</v>
       </c>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10">
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4">
         <v>102.0</v>
       </c>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="10"/>
-      <c r="Z19" s="10">
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4">
         <v>1.0</v>
       </c>
-      <c r="AA19" s="10"/>
-      <c r="AB19" s="10"/>
-      <c r="AC19" s="10"/>
-      <c r="AD19" s="10"/>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="10"/>
-      <c r="AG19" s="10"/>
-      <c r="AH19" s="10"/>
-      <c r="AI19" s="10"/>
-      <c r="AJ19" s="10"/>
-      <c r="AK19" s="10"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="4"/>
+      <c r="AG19" s="4"/>
+      <c r="AH19" s="4"/>
+      <c r="AI19" s="4"/>
+      <c r="AJ19" s="4"/>
+      <c r="AK19" s="4"/>
     </row>
     <row r="21" spans="1:37">
       <c r="A21" s="9" t="s">
-        <v>39</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="3"/>
+      <c r="AG21" s="3"/>
+      <c r="AH21" s="3"/>
+      <c r="AI21" s="3"/>
+      <c r="AJ21" s="3"/>
+      <c r="AK21" s="3"/>
     </row>
     <row r="22" spans="1:37">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N22" s="4" t="s">
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q22" s="4" t="s">
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="T22" s="4" t="s">
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="W22" s="4" t="s">
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Z22" s="4" t="s">
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AC22" s="4" t="s">
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AF22" s="4" t="s">
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI22" s="4" t="s">
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3"/>
     </row>
     <row r="23" spans="1:37">
-      <c r="B23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="U23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="V23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="X23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK23" s="3" t="s">
-        <v>37</v>
+      <c r="A23" s="3"/>
+      <c r="B23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="P23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="R23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="T23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="U23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="V23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="W23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="X23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK23" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:37">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="N24">
+      <c r="A24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3">
         <v>6.0</v>
       </c>
-      <c r="Q24">
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3">
         <v>10.0</v>
       </c>
-      <c r="T24">
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3">
         <v>57.0</v>
       </c>
-      <c r="W24">
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3">
         <v>63.0</v>
       </c>
-      <c r="Z24">
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3">
         <v>15.0</v>
       </c>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
     </row>
     <row r="25" spans="1:37">
-      <c r="A25" t="s">
-        <v>28</v>
-      </c>
+      <c r="A25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
     </row>
     <row r="26" spans="1:37">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z26">
+      <c r="A26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3">
         <v>1.0</v>
       </c>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
     </row>
     <row r="27" spans="1:37">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="3"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3"/>
     </row>
     <row r="28" spans="1:37">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3"/>
     </row>
     <row r="29" spans="1:37">
-      <c r="A29" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10">
+      <c r="A29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4">
         <v>6.0</v>
       </c>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10">
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4">
         <v>10.0</v>
       </c>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10">
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4">
         <v>57.0</v>
       </c>
-      <c r="U29" s="10"/>
-      <c r="V29" s="10"/>
-      <c r="W29" s="10">
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4">
         <v>63.0</v>
       </c>
-      <c r="X29" s="10"/>
-      <c r="Y29" s="10"/>
-      <c r="Z29" s="10">
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4">
         <v>16.0</v>
       </c>
-      <c r="AA29" s="10"/>
-      <c r="AB29" s="10"/>
-      <c r="AC29" s="10"/>
-      <c r="AD29" s="10"/>
-      <c r="AE29" s="10"/>
-      <c r="AF29" s="10"/>
-      <c r="AG29" s="10"/>
-      <c r="AH29" s="10"/>
-      <c r="AI29" s="10"/>
-      <c r="AJ29" s="10"/>
-      <c r="AK29" s="10"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4"/>
+      <c r="AI29" s="4"/>
+      <c r="AJ29" s="4"/>
+      <c r="AK29" s="4"/>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>